<commit_message>
nuevo cómputo de la tabla 2
</commit_message>
<xml_diff>
--- a/results/complete_Table2.xlsx
+++ b/results/complete_Table2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
   <si>
     <t>Parameter</t>
   </si>
@@ -117,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -127,14 +127,18 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -163,53 +167,53 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="K3">
@@ -223,7 +227,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="K4">
@@ -237,7 +241,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="K5">
@@ -251,7 +255,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="K6">
@@ -265,12 +269,12 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -280,14 +284,14 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0.012999999999999999</v>
+        <v>0.027</v>
       </c>
       <c r="K8">
         <v>0.10000000000000001</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -297,14 +301,14 @@
         <v>0.90000000000000002</v>
       </c>
       <c r="H9">
-        <v>0.98699999999999999</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="K9">
         <v>0.90000000000000002</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C10">
@@ -320,7 +324,7 @@
         <v>0.001</v>
       </c>
       <c r="I10">
-        <v>0.019</v>
+        <v>0.024</v>
       </c>
       <c r="J10">
         <v>0.108</v>
@@ -333,7 +337,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C11">
@@ -349,10 +353,10 @@
         <v>0.001</v>
       </c>
       <c r="I11">
-        <v>0.01</v>
+        <v>0.031</v>
       </c>
       <c r="J11">
-        <v>0.085000000000000006</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="L11">
         <v>0.14999999999999999</v>
@@ -362,7 +366,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C12">
@@ -372,14 +376,14 @@
         <v>0.84999999999999998</v>
       </c>
       <c r="I12">
-        <v>0.98099999999999998</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="L12">
         <v>0.84999999999999998</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C13">
@@ -389,14 +393,14 @@
         <v>0.84999999999999998</v>
       </c>
       <c r="I13">
-        <v>0.98999999999999999</v>
+        <v>0.96899999999999997</v>
       </c>
       <c r="L13">
         <v>0.84999999999999998</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D14">
@@ -413,7 +417,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H15">
@@ -427,12 +431,12 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B17">
@@ -454,13 +458,13 @@
         <v>-1017990117.132</v>
       </c>
       <c r="H17">
-        <v>-898981.77899999998</v>
+        <v>-1009688.6090000001</v>
       </c>
       <c r="I17">
-        <v>-898981.77899999998</v>
+        <v>-1009688.612</v>
       </c>
       <c r="J17">
-        <v>-471919.73800000001</v>
+        <v>-499773.44300000003</v>
       </c>
       <c r="K17">
         <v>-5964.6729999999998</v>
@@ -473,7 +477,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B18">
@@ -495,13 +499,13 @@
         <v>-872529715.80999994</v>
       </c>
       <c r="H18">
-        <v>-905739.58200000005</v>
+        <v>-983529.43299999996</v>
       </c>
       <c r="I18">
-        <v>-905739.58200000005</v>
+        <v>-983529.43599999999</v>
       </c>
       <c r="J18">
-        <v>-472587.44099999999</v>
+        <v>-489291.13299999997</v>
       </c>
       <c r="K18">
         <v>-4153.8540000000003</v>
@@ -514,7 +518,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B19">
@@ -536,13 +540,13 @@
         <v>1890513479.869</v>
       </c>
       <c r="H19">
-        <v>1780854.2620000001</v>
+        <v>1968630.6140000001</v>
       </c>
       <c r="I19">
-        <v>1780844.5349999999</v>
+        <v>1968630.3060000001</v>
       </c>
       <c r="J19">
-        <v>919516.22199999995</v>
+        <v>963236.42099999997</v>
       </c>
       <c r="K19">
         <v>871.09000000000003</v>
@@ -555,7 +559,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B20">
@@ -577,13 +581,13 @@
         <v>-6353.0730000000003</v>
       </c>
       <c r="H20">
-        <v>-23867.098000000002</v>
+        <v>-24587.429</v>
       </c>
       <c r="I20">
-        <v>-23876.825000000001</v>
+        <v>-24587.741000000002</v>
       </c>
       <c r="J20">
-        <v>-24990.956999999999</v>
+        <v>-25828.155999999999</v>
       </c>
       <c r="K20">
         <v>-9247.4359999999997</v>

</xml_diff>

<commit_message>
implemento muchos cambios para hacer funcionar la tabla 5, todavía no he terminado
</commit_message>
<xml_diff>
--- a/results/complete_Table2.xlsx
+++ b/results/complete_Table2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="28">
   <si>
     <t>Parameter</t>
   </si>
@@ -117,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -129,16 +129,20 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -167,53 +171,53 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="K3">
@@ -227,7 +231,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="K4">
@@ -241,7 +245,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="K5">
@@ -255,7 +259,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="K6">
@@ -269,12 +273,12 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -291,7 +295,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -308,7 +312,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C10">
@@ -337,7 +341,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C11">
@@ -366,7 +370,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C12">
@@ -383,7 +387,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C13">
@@ -400,7 +404,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D14">
@@ -417,7 +421,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H15">
@@ -431,12 +435,12 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B17">
@@ -477,7 +481,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B18">
@@ -518,7 +522,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B19">
@@ -559,7 +563,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B20">

</xml_diff>

<commit_message>
la verdad muchos cambios, todavía esto no termina. Cambios para hacer funcionar la tabla 5 y cambios para que log-ll de más cercano en todos los modelos, y cambios en las restricciones para que los parámetros tengan variabilidad
</commit_message>
<xml_diff>
--- a/results/complete_Table2.xlsx
+++ b/results/complete_Table2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="28">
   <si>
     <t>Parameter</t>
   </si>
@@ -117,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -131,11 +131,51 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -143,6 +183,46 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -161,7 +241,7 @@
     <col min="4" max="4" width="9.33203125" customWidth="true"/>
     <col min="5" max="5" width="14" customWidth="true"/>
     <col min="6" max="6" width="16.21875" customWidth="true"/>
-    <col min="7" max="7" width="12.21875" customWidth="true"/>
+    <col min="7" max="7" width="11.21875" customWidth="true"/>
     <col min="8" max="8" width="15.21875" customWidth="true"/>
     <col min="9" max="9" width="17.44140625" customWidth="true"/>
     <col min="10" max="10" width="12.44140625" customWidth="true"/>
@@ -171,53 +251,53 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="45" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="45" t="s">
         <v>2</v>
       </c>
       <c r="K3">
@@ -231,7 +311,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="45" t="s">
         <v>3</v>
       </c>
       <c r="K4">
@@ -245,7 +325,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="45" t="s">
         <v>4</v>
       </c>
       <c r="K5">
@@ -259,7 +339,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
       <c r="K6">
@@ -273,104 +353,104 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="45" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="45" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>0.039</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.039</v>
       </c>
       <c r="H8">
-        <v>0.027</v>
+        <v>0.039</v>
       </c>
       <c r="K8">
-        <v>0.10000000000000001</v>
+        <v>0.039</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="45" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.90000000000000002</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="E9">
-        <v>0.90000000000000002</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="H9">
-        <v>0.97299999999999998</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="K9">
-        <v>0.90000000000000002</v>
+        <v>0.29999999999999999</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="45" t="s">
         <v>2</v>
       </c>
       <c r="C10">
-        <v>0.001</v>
+        <v>0.039</v>
       </c>
       <c r="D10">
-        <v>0.019</v>
+        <v>0.039</v>
       </c>
       <c r="F10">
-        <v>0.001</v>
+        <v>0.039</v>
       </c>
       <c r="G10">
-        <v>0.001</v>
+        <v>0.039</v>
       </c>
       <c r="I10">
-        <v>0.024</v>
+        <v>0.039</v>
       </c>
       <c r="J10">
-        <v>0.108</v>
+        <v>0.039</v>
       </c>
       <c r="L10">
-        <v>0.14999999999999999</v>
+        <v>0.040000000000000001</v>
       </c>
       <c r="M10">
-        <v>0.98699999999999999</v>
+        <v>0.040000000000000001</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="45" t="s">
         <v>4</v>
       </c>
       <c r="C11">
-        <v>0.001</v>
+        <v>0.039</v>
       </c>
       <c r="D11">
-        <v>0.02</v>
+        <v>0.039</v>
       </c>
       <c r="F11">
-        <v>0.001</v>
+        <v>0.039</v>
       </c>
       <c r="G11">
-        <v>0.001</v>
+        <v>0.039</v>
       </c>
       <c r="I11">
-        <v>0.031</v>
+        <v>0.039</v>
       </c>
       <c r="J11">
-        <v>0.11600000000000001</v>
+        <v>0.039</v>
       </c>
       <c r="L11">
-        <v>0.14999999999999999</v>
+        <v>0.040000000000000001</v>
       </c>
       <c r="M11">
-        <v>0.10000000000000001</v>
+        <v>0.040000000000000001</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="45" t="s">
         <v>3</v>
       </c>
       <c r="C12">
@@ -380,14 +460,14 @@
         <v>0.84999999999999998</v>
       </c>
       <c r="I12">
-        <v>0.97599999999999998</v>
+        <v>0.84999999999999998</v>
       </c>
       <c r="L12">
-        <v>0.84999999999999998</v>
+        <v>0.91300000000000003</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="45" t="s">
         <v>5</v>
       </c>
       <c r="C13">
@@ -397,210 +477,210 @@
         <v>0.84999999999999998</v>
       </c>
       <c r="I13">
-        <v>0.96899999999999997</v>
+        <v>0.84999999999999998</v>
       </c>
       <c r="L13">
-        <v>0.84999999999999998</v>
+        <v>0.91300000000000003</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="45" t="s">
         <v>9</v>
       </c>
       <c r="D14">
-        <v>0.02</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="G14">
-        <v>0.001</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="J14">
-        <v>0.98999999999999999</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="M14">
-        <v>0.98699999999999999</v>
+        <v>0.89000000000000001</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="45" t="s">
         <v>10</v>
       </c>
       <c r="H15">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>0.01</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="45" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="45" t="s">
         <v>12</v>
       </c>
       <c r="B17">
-        <v>-2996.9670000000001</v>
+        <v>-2912.6759999999999</v>
       </c>
       <c r="C17">
-        <v>-2996.9670000000001</v>
+        <v>-2912.6759999999999</v>
       </c>
       <c r="D17">
-        <v>-2921.6729999999998</v>
+        <v>-2912.6759999999999</v>
       </c>
       <c r="E17">
-        <v>-3085.4839999999999</v>
+        <v>-10580.528</v>
       </c>
       <c r="F17">
-        <v>-3111.5859999999998</v>
+        <v>-3061.8620000000001</v>
       </c>
       <c r="G17">
-        <v>-1017990117.132</v>
+        <v>-3042.0880000000002</v>
       </c>
       <c r="H17">
-        <v>-1009688.6090000001</v>
+        <v>-3226.5590000000002</v>
       </c>
       <c r="I17">
-        <v>-1009688.612</v>
+        <v>-3226.5590000000002</v>
       </c>
       <c r="J17">
-        <v>-499773.44300000003</v>
+        <v>-3226.5590000000002</v>
       </c>
       <c r="K17">
-        <v>-5964.6729999999998</v>
+        <v>-6140.8270000000002</v>
       </c>
       <c r="L17">
-        <v>-5964.6729999999998</v>
+        <v>-6140.8270000000002</v>
       </c>
       <c r="M17">
-        <v>-5964.6729999999998</v>
+        <v>-6140.8270000000002</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="45" t="s">
         <v>13</v>
       </c>
       <c r="B18">
-        <v>-3019.502</v>
+        <v>-2963.6080000000002</v>
       </c>
       <c r="C18">
-        <v>-3019.502</v>
+        <v>-2963.6080000000002</v>
       </c>
       <c r="D18">
-        <v>-2982.085</v>
+        <v>-2963.6080000000002</v>
       </c>
       <c r="E18">
-        <v>-2934.8400000000001</v>
+        <v>-8960.7530000000006</v>
       </c>
       <c r="F18">
-        <v>-2943.9859999999999</v>
+        <v>-2832.7220000000002</v>
       </c>
       <c r="G18">
-        <v>-872529715.80999994</v>
+        <v>-2829.9290000000001</v>
       </c>
       <c r="H18">
-        <v>-983529.43299999996</v>
+        <v>-3223.9200000000001</v>
       </c>
       <c r="I18">
-        <v>-983529.43599999999</v>
+        <v>-3223.9200000000001</v>
       </c>
       <c r="J18">
-        <v>-489291.13299999997</v>
+        <v>-3223.9200000000001</v>
       </c>
       <c r="K18">
-        <v>-4153.8540000000003</v>
+        <v>-4358.2759999999998</v>
       </c>
       <c r="L18">
-        <v>-4153.8540000000003</v>
+        <v>-4358.2759999999998</v>
       </c>
       <c r="M18">
-        <v>-4153.8540000000003</v>
+        <v>-4358.2759999999998</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="45" t="s">
         <v>14</v>
       </c>
       <c r="B19">
-        <v>-337.62299999999999</v>
+        <v>-286.76499999999999</v>
       </c>
       <c r="C19">
-        <v>-304.78699999999998</v>
+        <v>-5.5309999999999997</v>
       </c>
       <c r="D19">
-        <v>-373.274</v>
+        <v>-5.5309999999999997</v>
       </c>
       <c r="E19">
-        <v>-333.76799999999997</v>
+        <v>13358.513000000001</v>
       </c>
       <c r="F19">
-        <v>-265.68400000000003</v>
+        <v>-10.598000000000001</v>
       </c>
       <c r="G19">
-        <v>1890513479.869</v>
+        <v>-33.165999999999997</v>
       </c>
       <c r="H19">
-        <v>1968630.6140000001</v>
+        <v>287.43000000000001</v>
       </c>
       <c r="I19">
-        <v>1968630.3060000001</v>
+        <v>568.66300000000001</v>
       </c>
       <c r="J19">
-        <v>963236.42099999997</v>
+        <v>568.66300000000001</v>
       </c>
       <c r="K19">
-        <v>871.09000000000003</v>
+        <v>-0</v>
       </c>
       <c r="L19">
-        <v>747.64300000000003</v>
+        <v>-0</v>
       </c>
       <c r="M19">
-        <v>-514.63800000000003</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="45" t="s">
         <v>15</v>
       </c>
       <c r="B20">
-        <v>-6354.0919999999996</v>
+        <v>-6163.049</v>
       </c>
       <c r="C20">
-        <v>-6321.2560000000003</v>
+        <v>-5881.8149999999996</v>
       </c>
       <c r="D20">
-        <v>-6277.0320000000002</v>
+        <v>-5881.8149999999996</v>
       </c>
       <c r="E20">
-        <v>-6354.0919999999996</v>
+        <v>-6182.768</v>
       </c>
       <c r="F20">
-        <v>-6321.2560000000003</v>
+        <v>-5905.1819999999998</v>
       </c>
       <c r="G20">
-        <v>-6353.0730000000003</v>
+        <v>-5905.1819999999998</v>
       </c>
       <c r="H20">
-        <v>-24587.429</v>
+        <v>-6163.049</v>
       </c>
       <c r="I20">
-        <v>-24587.741000000002</v>
+        <v>-5881.8149999999996</v>
       </c>
       <c r="J20">
-        <v>-25828.155999999999</v>
+        <v>-5881.8149999999996</v>
       </c>
       <c r="K20">
-        <v>-9247.4359999999997</v>
+        <v>-10499.102000000001</v>
       </c>
       <c r="L20">
-        <v>-9370.8829999999998</v>
+        <v>-10499.102000000001</v>
       </c>
       <c r="M20">
-        <v>-10633.165000000001</v>
+        <v>-10499.102000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solucionado el problema de la indexación, tabla generada con éxito
</commit_message>
<xml_diff>
--- a/results/complete_Table2.xlsx
+++ b/results/complete_Table2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="28">
   <si>
     <t>Parameter</t>
   </si>
@@ -117,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="63">
+  <borders count="65">
     <border>
       <left/>
       <right/>
@@ -187,11 +187,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -255,6 +257,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -271,448 +275,292 @@
     <col min="2" max="2" width="12.109375" customWidth="true"/>
     <col min="3" max="3" width="14.33203125" customWidth="true"/>
     <col min="4" max="4" width="9.33203125" customWidth="true"/>
-    <col min="5" max="5" width="16.21875" customWidth="true"/>
+    <col min="5" max="5" width="14" customWidth="true"/>
     <col min="6" max="6" width="16.21875" customWidth="true"/>
-    <col min="7" max="7" width="12.21875" customWidth="true"/>
-    <col min="8" max="8" width="16.21875" customWidth="true"/>
+    <col min="7" max="7" width="11.21875" customWidth="true"/>
+    <col min="8" max="8" width="15.21875" customWidth="true"/>
     <col min="9" max="9" width="17.44140625" customWidth="true"/>
-    <col min="10" max="10" width="16.21875" customWidth="true"/>
+    <col min="10" max="10" width="12.44140625" customWidth="true"/>
     <col min="11" max="11" width="11.44140625" customWidth="true"/>
     <col min="12" max="12" width="13.6640625" customWidth="true"/>
-    <col min="13" max="13" width="11.21875" customWidth="true"/>
+    <col min="13" max="13" width="8.6640625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="F1" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="G1" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="61" t="s">
+      <c r="H1" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="61" t="s">
+      <c r="J1" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="61" t="s">
+      <c r="K1" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="61" t="s">
+      <c r="L1" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="61" t="s">
+      <c r="M1" s="63" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="63" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="63" t="s">
         <v>2</v>
       </c>
       <c r="K3">
         <v>0.079000000000000001</v>
       </c>
-      <c r="L3">
-        <v>0.079000000000000001</v>
-      </c>
-      <c r="M3">
-        <v>0.079000000000000001</v>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="63" t="s">
         <v>3</v>
       </c>
       <c r="K4">
-        <v>0.89900000000000002</v>
-      </c>
-      <c r="L4">
-        <v>0.89900000000000002</v>
-      </c>
-      <c r="M4">
-        <v>0.89900000000000002</v>
+        <v>0.90000000000000002</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="63" t="s">
         <v>4</v>
       </c>
       <c r="K5">
-        <v>0.045999999999999999</v>
-      </c>
-      <c r="L5">
-        <v>0.045999999999999999</v>
-      </c>
-      <c r="M5">
-        <v>0.045999999999999999</v>
+        <v>0.047</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="63" t="s">
         <v>5</v>
       </c>
       <c r="K6">
-        <v>0.94699999999999995</v>
-      </c>
-      <c r="L6">
-        <v>0.94699999999999995</v>
-      </c>
-      <c r="M6">
-        <v>0.94699999999999995</v>
+        <v>0.94599999999999995</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="63" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="63" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.001</v>
-      </c>
-      <c r="E8">
-        <v>0.001</v>
-      </c>
-      <c r="H8">
-        <v>0.001</v>
+        <v>0.223</v>
       </c>
       <c r="K8">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="63" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="K9">
+        <v>0.97699999999999998</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="D10">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="I10">
+        <v>0.88400000000000001</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>0.19</v>
+      </c>
+      <c r="D11">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="F11">
+        <v>-0</v>
+      </c>
+      <c r="I11">
         <v>1</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="61" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="61" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>0.001</v>
-      </c>
-      <c r="D10">
-        <v>0.001</v>
-      </c>
-      <c r="F10">
-        <v>0.001</v>
-      </c>
-      <c r="G10">
-        <v>0.001</v>
-      </c>
-      <c r="I10">
-        <v>0.001</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>0.96499999999999997</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="61" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>0.001</v>
-      </c>
-      <c r="D11">
-        <v>0.001</v>
-      </c>
-      <c r="F11">
-        <v>0.001</v>
-      </c>
-      <c r="G11">
-        <v>0.001</v>
-      </c>
-      <c r="I11">
-        <v>0.001</v>
-      </c>
-      <c r="J11">
-        <v>0.001</v>
-      </c>
-      <c r="L11">
-        <v>0.045999999999999999</v>
-      </c>
-      <c r="M11">
-        <v>0.59899999999999998</v>
-      </c>
-    </row>
     <row r="12">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="63" t="s">
         <v>3</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.95399999999999996</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.082000000000000003</v>
       </c>
       <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
+        <v>0.041000000000000002</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="63" t="s">
         <v>5</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.97999999999999998</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>0.059999999999999998</v>
       </c>
       <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0.95399999999999996</v>
+        <v>0.087999999999999995</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="63" t="s">
         <v>9</v>
       </c>
       <c r="D14">
-        <v>0.001</v>
-      </c>
-      <c r="G14">
-        <v>0.001</v>
-      </c>
-      <c r="J14">
-        <v>0.001</v>
-      </c>
-      <c r="M14">
-        <v>0.93000000000000005</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="61" t="s">
+      <c r="A15" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="H15">
-        <v>26395786.563999999</v>
-      </c>
-      <c r="I15">
-        <v>158823959453.832</v>
-      </c>
-      <c r="J15">
-        <v>604152.47400000005</v>
-      </c>
     </row>
     <row r="16">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="63" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="63" t="s">
         <v>12</v>
       </c>
       <c r="B17">
-        <v>-3040.663</v>
+        <v>-5604.1139999999996</v>
       </c>
       <c r="C17">
-        <v>-3040.663</v>
+        <v>-5595.8299999999999</v>
       </c>
       <c r="D17">
-        <v>-3040.663</v>
-      </c>
-      <c r="E17">
-        <v>-2.4837757804260102e+19</v>
+        <v>-5603.2150000000001</v>
       </c>
       <c r="F17">
-        <v>-642816299984447.63</v>
-      </c>
-      <c r="G17">
-        <v>-4110140134.9749999</v>
-      </c>
-      <c r="H17">
-        <v>-40289.911</v>
+        <v>-5643.6319999999996</v>
       </c>
       <c r="I17">
-        <v>-59791.870999999999</v>
-      </c>
-      <c r="J17">
-        <v>-31825.356</v>
+        <v>-5619.1949999999997</v>
       </c>
       <c r="K17">
-        <v>-4358.2759999999998</v>
-      </c>
-      <c r="L17">
-        <v>-4358.2759999999998</v>
-      </c>
-      <c r="M17">
-        <v>-4358.2759999999998</v>
+        <v>-8805.7099999999991</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="63" t="s">
         <v>13</v>
       </c>
       <c r="B18">
-        <v>-5850.9740000000002</v>
+        <v>-5604.1139999999996</v>
       </c>
       <c r="C18">
-        <v>-5850.9740000000002</v>
+        <v>-5595.8299999999999</v>
       </c>
       <c r="D18">
-        <v>-5850.9740000000002</v>
-      </c>
-      <c r="E18">
-        <v>-1.2876704058346458e+18</v>
+        <v>-5603.2150000000001</v>
       </c>
       <c r="F18">
-        <v>-33325694362915.898</v>
-      </c>
-      <c r="G18">
-        <v>-213070287.54800001</v>
-      </c>
-      <c r="H18">
-        <v>-40292.332999999999</v>
+        <v>-5643.6319999999996</v>
       </c>
       <c r="I18">
-        <v>-59794.294000000002</v>
-      </c>
-      <c r="J18">
-        <v>-31827.777999999998</v>
+        <v>-5619.1949999999997</v>
       </c>
       <c r="K18">
-        <v>-6140.8270000000002</v>
-      </c>
-      <c r="L18">
-        <v>-6140.8270000000002</v>
-      </c>
-      <c r="M18">
-        <v>-6140.8270000000002</v>
+        <v>-8805.7099999999991</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="61" t="s">
+      <c r="A19" s="63" t="s">
         <v>14</v>
       </c>
       <c r="B19">
-        <v>-4665.2290000000003</v>
+        <v>-5604.1139999999996</v>
       </c>
       <c r="C19">
-        <v>-4665.2280000000001</v>
+        <v>-5595.8299999999999</v>
       </c>
       <c r="D19">
-        <v>-4665.2290000000003</v>
-      </c>
-      <c r="E19">
-        <v>2.6125428210094735e+19</v>
+        <v>-5603.2150000000001</v>
       </c>
       <c r="F19">
-        <v>676141994333837.75</v>
-      </c>
-      <c r="G19">
-        <v>4323196896.7399998</v>
-      </c>
-      <c r="H19">
-        <v>-333023134886763.25</v>
+        <v>-5643.6319999999996</v>
       </c>
       <c r="I19">
-        <v>-1.203990936401597e+22</v>
-      </c>
-      <c r="J19">
-        <v>-2418838071769538.5</v>
+        <v>-5619.1949999999997</v>
       </c>
       <c r="K19">
-        <v>-26155.835999999999</v>
-      </c>
-      <c r="L19">
-        <v>-41050.481</v>
-      </c>
-      <c r="M19">
-        <v>-4238389.3300000001</v>
+        <v>-8805.7099999999991</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="63" t="s">
         <v>15</v>
       </c>
       <c r="B20">
-        <v>-13556.865</v>
+        <v>-5604.1139999999996</v>
       </c>
       <c r="C20">
-        <v>-13556.865</v>
+        <v>-5595.8299999999999</v>
       </c>
       <c r="D20">
-        <v>-13556.865</v>
-      </c>
-      <c r="E20">
-        <v>-13525.782999999999</v>
+        <v>-5603.2150000000001</v>
       </c>
       <c r="F20">
-        <v>-13525.782999999999</v>
-      </c>
-      <c r="G20">
-        <v>-13525.782999999999</v>
-      </c>
-      <c r="H20">
-        <v>-333023134967345.5</v>
+        <v>-5643.6319999999996</v>
       </c>
       <c r="I20">
-        <v>-1.203990936401597e+22</v>
-      </c>
-      <c r="J20">
-        <v>-2418838071833191.5</v>
+        <v>-5619.1949999999997</v>
       </c>
       <c r="K20">
-        <v>-36654.938000000002</v>
-      </c>
-      <c r="L20">
-        <v>-51549.582999999999</v>
-      </c>
-      <c r="M20">
-        <v>-4248888.432</v>
+        <v>-8805.7099999999991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ya me cansé de Asymdata y g,l, o y todas las yerbas que no usare, las estoy sacando de rdcc.m y de rdcc_likelihood.m. Gracias ya termino, yo te aviso
</commit_message>
<xml_diff>
--- a/results/complete_Table2.xlsx
+++ b/results/complete_Table2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="28">
   <si>
     <t>Parameter</t>
   </si>
@@ -117,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="65">
+  <borders count="67">
     <border>
       <left/>
       <right/>
@@ -189,11 +189,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -259,6 +261,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -287,90 +291,114 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="63" t="s">
+      <c r="G1" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="63" t="s">
+      <c r="H1" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="63" t="s">
+      <c r="I1" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="63" t="s">
+      <c r="J1" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="63" t="s">
+      <c r="K1" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="63" t="s">
+      <c r="L1" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="63" t="s">
+      <c r="M1" s="65" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="65" t="s">
         <v>2</v>
       </c>
       <c r="K3">
         <v>0.079000000000000001</v>
       </c>
+      <c r="L3">
+        <v>0.079000000000000001</v>
+      </c>
+      <c r="M3">
+        <v>0.079000000000000001</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="65" t="s">
         <v>3</v>
       </c>
       <c r="K4">
-        <v>0.90000000000000002</v>
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="L4">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="M4">
+        <v>0.89900000000000002</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="65" t="s">
         <v>4</v>
       </c>
       <c r="K5">
-        <v>0.047</v>
+        <v>0.045999999999999999</v>
+      </c>
+      <c r="L5">
+        <v>0.045999999999999999</v>
+      </c>
+      <c r="M5">
+        <v>0.045999999999999999</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="65" t="s">
         <v>5</v>
       </c>
       <c r="K6">
-        <v>0.94599999999999995</v>
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="L6">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="M6">
+        <v>0.94699999999999995</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="65" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="65" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -381,7 +409,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="65" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -392,7 +420,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="63" t="s">
+      <c r="A10" s="65" t="s">
         <v>2</v>
       </c>
       <c r="C10">
@@ -409,7 +437,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="65" t="s">
         <v>4</v>
       </c>
       <c r="C11">
@@ -426,7 +454,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="65" t="s">
         <v>3</v>
       </c>
       <c r="C12">
@@ -440,7 +468,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="65" t="s">
         <v>5</v>
       </c>
       <c r="C13">
@@ -454,7 +482,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="63" t="s">
+      <c r="A14" s="65" t="s">
         <v>9</v>
       </c>
       <c r="D14">
@@ -462,17 +490,17 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="65" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="65" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="65" t="s">
         <v>12</v>
       </c>
       <c r="B17">
@@ -495,7 +523,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="63" t="s">
+      <c r="A18" s="65" t="s">
         <v>13</v>
       </c>
       <c r="B18">
@@ -518,7 +546,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="65" t="s">
         <v>14</v>
       </c>
       <c r="B19">
@@ -541,7 +569,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="65" t="s">
         <v>15</v>
       </c>
       <c r="B20">

</xml_diff>

<commit_message>
pormenorizadas las modificaciones sobre los vectores a y b para que la multiplicación por los errores cuadráticos y covarianzas condicionales pasadas sea correcto
</commit_message>
<xml_diff>
--- a/results/complete_Table2.xlsx
+++ b/results/complete_Table2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="28">
   <si>
     <t>Parameter</t>
   </si>
@@ -117,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="67">
+  <borders count="81">
     <border>
       <left/>
       <right/>
@@ -191,11 +191,25 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -263,6 +277,20 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="67" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="68" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="69" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="70" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="71" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="72" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="73" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="74" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="75" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="76" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="77" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="78" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="79" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -287,57 +315,57 @@
     <col min="10" max="10" width="12.44140625" customWidth="true"/>
     <col min="11" max="11" width="11.44140625" customWidth="true"/>
     <col min="12" max="12" width="13.6640625" customWidth="true"/>
-    <col min="13" max="13" width="8.6640625" customWidth="true"/>
+    <col min="13" max="13" width="9.6640625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="E1" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="65" t="s">
+      <c r="F1" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="65" t="s">
+      <c r="G1" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="65" t="s">
+      <c r="H1" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="65" t="s">
+      <c r="I1" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="65" t="s">
+      <c r="J1" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="65" t="s">
+      <c r="K1" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="65" t="s">
+      <c r="L1" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="65" t="s">
+      <c r="M1" s="79" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="79" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
       <c r="K3">
@@ -351,7 +379,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
       <c r="K4">
@@ -365,7 +393,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="79" t="s">
         <v>4</v>
       </c>
       <c r="K5">
@@ -379,7 +407,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="79" t="s">
         <v>5</v>
       </c>
       <c r="K6">
@@ -393,34 +421,34 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="79" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="79" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <v>0.223</v>
       </c>
       <c r="K8">
-        <v>0.012</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="79" t="s">
         <v>8</v>
       </c>
       <c r="B9">
         <v>0.97099999999999997</v>
       </c>
       <c r="K9">
-        <v>0.97699999999999998</v>
+        <v>0.98599999999999999</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="79" t="s">
         <v>2</v>
       </c>
       <c r="C10">
@@ -435,9 +463,15 @@
       <c r="I10">
         <v>0.88400000000000001</v>
       </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0.0050000000000000001</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="79" t="s">
         <v>4</v>
       </c>
       <c r="C11">
@@ -452,9 +486,15 @@
       <c r="I11">
         <v>1</v>
       </c>
+      <c r="L11">
+        <v>0.02</v>
+      </c>
+      <c r="M11">
+        <v>0.0050000000000000001</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="79" t="s">
         <v>3</v>
       </c>
       <c r="C12">
@@ -466,9 +506,12 @@
       <c r="I12">
         <v>0.041000000000000002</v>
       </c>
+      <c r="L12">
+        <v>0.52000000000000002</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="79" t="s">
         <v>5</v>
       </c>
       <c r="C13">
@@ -480,27 +523,33 @@
       <c r="I13">
         <v>0.087999999999999995</v>
       </c>
+      <c r="L13">
+        <v>0.63500000000000001</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="65" t="s">
+      <c r="A14" s="79" t="s">
         <v>9</v>
       </c>
       <c r="D14">
         <v>0.997</v>
       </c>
+      <c r="M14">
+        <v>0.495</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="79" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="65" t="s">
+      <c r="A16" s="79" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="65" t="s">
+      <c r="A17" s="79" t="s">
         <v>12</v>
       </c>
       <c r="B17">
@@ -519,11 +568,17 @@
         <v>-5619.1949999999997</v>
       </c>
       <c r="K17">
-        <v>-8805.7099999999991</v>
+        <v>-8821.7430000000004</v>
+      </c>
+      <c r="L17">
+        <v>-10000000</v>
+      </c>
+      <c r="M17">
+        <v>-10000000</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="79" t="s">
         <v>13</v>
       </c>
       <c r="B18">
@@ -542,11 +597,17 @@
         <v>-5619.1949999999997</v>
       </c>
       <c r="K18">
-        <v>-8805.7099999999991</v>
+        <v>-8821.7430000000004</v>
+      </c>
+      <c r="L18">
+        <v>-10000000</v>
+      </c>
+      <c r="M18">
+        <v>-10000000</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="79" t="s">
         <v>14</v>
       </c>
       <c r="B19">
@@ -565,11 +626,17 @@
         <v>-5619.1949999999997</v>
       </c>
       <c r="K19">
-        <v>-8805.7099999999991</v>
+        <v>-8821.7430000000004</v>
+      </c>
+      <c r="L19">
+        <v>-10000000</v>
+      </c>
+      <c r="M19">
+        <v>-10000000</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="65" t="s">
+      <c r="A20" s="79" t="s">
         <v>15</v>
       </c>
       <c r="B20">
@@ -588,7 +655,13 @@
         <v>-5619.1949999999997</v>
       </c>
       <c r="K20">
-        <v>-8805.7099999999991</v>
+        <v>-8821.7430000000004</v>
+      </c>
+      <c r="L20">
+        <v>-10000000</v>
+      </c>
+      <c r="M20">
+        <v>-10000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>